<commit_message>
Added Component Values for the AC Voltage sensor
</commit_message>
<xml_diff>
--- a/Hardware/Component Values.xlsx
+++ b/Hardware/Component Values.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="9555" windowHeight="10815" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="9555" windowHeight="10815"/>
   </bookViews>
   <sheets>
     <sheet name="AC Voltage" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>Component</t>
   </si>
@@ -136,6 +136,18 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>SD103</t>
+  </si>
+  <si>
+    <t>100nF</t>
   </si>
 </sst>
 </file>
@@ -251,6 +263,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>455519</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>111498</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>367846</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>44093</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="455519" y="2968998"/>
+          <a:ext cx="15533327" cy="5838095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -542,9 +597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3:L6"/>
+      <selection pane="bottomLeft" activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +681,7 @@
         <v>0.35</v>
       </c>
       <c r="I3" s="5">
-        <f t="shared" ref="I3:I17" si="0">H3*G3</f>
+        <f t="shared" ref="I3:I14" si="0">H3*G3</f>
         <v>1.0499999999999998</v>
       </c>
       <c r="K3" s="6" t="s">
@@ -647,6 +702,12 @@
       <c r="C4" t="s">
         <v>26</v>
       </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
       <c r="H4" s="5">
         <v>0</v>
       </c>
@@ -691,7 +752,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="H6" s="5">
         <v>0</v>
@@ -723,7 +784,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -800,6 +861,9 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="C13" t="s">
         <v>19</v>
       </c>
@@ -823,6 +887,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -981,7 +1046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated the Main Board
Main Board is Fully Done. need to Test the timing circuit before sending
the design for manufacture
</commit_message>
<xml_diff>
--- a/Hardware/Component Values.xlsx
+++ b/Hardware/Component Values.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="9555" windowHeight="10815"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="9555" windowHeight="10815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AC Voltage" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
   <si>
     <t>Component</t>
   </si>
@@ -148,6 +148,27 @@
   </si>
   <si>
     <t>100nF</t>
+  </si>
+  <si>
+    <t>1n</t>
+  </si>
+  <si>
+    <t>100n</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>1.5k</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>ACS712</t>
+  </si>
+  <si>
+    <t>MCP601</t>
   </si>
 </sst>
 </file>
@@ -297,6 +318,49 @@
         <a:xfrm>
           <a:off x="455519" y="2968998"/>
           <a:ext cx="15533327" cy="5838095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>157334</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>106090</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>6628</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3586334"/>
+          <a:ext cx="14931472" cy="4802294"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -597,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U7" sqref="U7"/>
     </sheetView>
@@ -969,11 +1033,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,7 +1075,33 @@
         <v>35</v>
       </c>
     </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
       <c r="K3" s="6" t="s">
         <v>34</v>
       </c>
@@ -1021,6 +1111,12 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
       <c r="K4" s="6" t="s">
         <v>32</v>
       </c>
@@ -1029,6 +1125,12 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
       <c r="K5" s="6" t="s">
         <v>33</v>
       </c>
@@ -1037,8 +1139,41 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>